<commit_message>
minopen aanpassing + pv_distance
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -487,22 +487,22 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -532,7 +532,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -567,12 +567,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-0.0</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -612,7 +612,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -647,12 +647,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-0.0</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -687,12 +687,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>-0.0</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -732,7 +732,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -772,7 +772,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -812,7 +812,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -847,12 +847,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-0.0</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -887,12 +887,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-0.0</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -927,12 +927,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-0.0</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -967,27 +967,27 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1007,27 +1007,27 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1047,27 +1047,27 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1087,27 +1087,27 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1132,22 +1132,22 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1167,27 +1167,27 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1207,27 +1207,27 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1247,27 +1247,27 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1287,27 +1287,27 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1332,22 +1332,22 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1367,27 +1367,27 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1412,22 +1412,22 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1447,27 +1447,27 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1487,27 +1487,27 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1527,27 +1527,27 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1567,27 +1567,27 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1612,22 +1612,22 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1647,27 +1647,27 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1687,27 +1687,27 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1727,27 +1727,27 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1767,27 +1767,27 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1812,22 +1812,22 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1847,27 +1847,27 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1892,22 +1892,22 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1927,27 +1927,27 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -1967,27 +1967,27 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2007,27 +2007,27 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2047,27 +2047,27 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2092,22 +2092,22 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2127,27 +2127,27 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2167,27 +2167,27 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2207,27 +2207,27 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2247,27 +2247,27 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2292,22 +2292,22 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2327,27 +2327,27 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2372,22 +2372,22 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2407,27 +2407,27 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2452,17 +2452,17 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -2487,27 +2487,27 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2527,27 +2527,27 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2572,22 +2572,22 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2607,27 +2607,27 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2647,27 +2647,27 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2687,27 +2687,27 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2727,27 +2727,27 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2772,22 +2772,22 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2807,27 +2807,27 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2852,22 +2852,22 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2887,27 +2887,27 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2927,27 +2927,27 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2967,27 +2967,27 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3007,17 +3007,17 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
@@ -3027,7 +3027,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3052,22 +3052,22 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3087,27 +3087,27 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3127,27 +3127,27 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3167,27 +3167,27 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3207,27 +3207,27 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3252,22 +3252,22 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3287,27 +3287,27 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3332,22 +3332,22 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3367,27 +3367,27 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3407,27 +3407,27 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3447,27 +3447,27 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3487,27 +3487,27 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3532,22 +3532,22 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3567,27 +3567,27 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3607,12 +3607,12 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>24.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -3622,12 +3622,12 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3647,27 +3647,27 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3687,27 +3687,27 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3732,22 +3732,22 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3767,27 +3767,27 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3812,22 +3812,22 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3847,27 +3847,27 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3887,27 +3887,27 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3927,27 +3927,27 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -3967,27 +3967,27 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4012,22 +4012,22 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4047,27 +4047,27 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4087,27 +4087,27 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4127,27 +4127,27 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>14.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>9.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>9.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4167,27 +4167,27 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4212,22 +4212,22 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4247,27 +4247,27 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4292,22 +4292,22 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4327,27 +4327,27 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4367,27 +4367,27 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4407,27 +4407,27 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4447,27 +4447,27 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4492,22 +4492,22 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4527,27 +4527,27 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4567,27 +4567,27 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4607,27 +4607,27 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4647,27 +4647,27 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4692,22 +4692,22 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4727,27 +4727,27 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4772,22 +4772,22 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H109" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4807,27 +4807,27 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4847,27 +4847,27 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4887,27 +4887,27 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4927,27 +4927,27 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -4972,22 +4972,22 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5007,27 +5007,27 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5047,27 +5047,27 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5087,27 +5087,27 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H117" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5127,27 +5127,27 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5172,22 +5172,22 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5207,27 +5207,27 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5252,22 +5252,22 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5287,27 +5287,27 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5327,27 +5327,27 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5367,27 +5367,27 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5407,27 +5407,27 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5452,22 +5452,22 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5487,27 +5487,27 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5527,27 +5527,27 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5567,27 +5567,27 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5607,27 +5607,27 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5652,22 +5652,22 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5687,22 +5687,22 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H132" t="inlineStr">
@@ -5732,22 +5732,22 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5767,27 +5767,27 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5807,27 +5807,27 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5847,27 +5847,27 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5887,27 +5887,27 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5932,22 +5932,22 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -5967,27 +5967,27 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H139" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -6007,27 +6007,27 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H140" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -6047,27 +6047,27 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H141" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -6087,27 +6087,27 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -6132,22 +6132,22 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H143" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -6167,27 +6167,27 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H144" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -6212,22 +6212,22 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H145" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>

</xml_diff>